<commit_message>
change 3 folder and add 1
</commit_message>
<xml_diff>
--- a/配置管理/0514/配置项计划表.xlsx
+++ b/配置管理/0514/配置项计划表.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="12780" windowHeight="11640" tabRatio="498" activeTab="1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
   <si>
     <t>数据形式</t>
   </si>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>项目开始的依据</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>提示：</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -120,20 +116,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>项目管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>工程过程</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>项目支撑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求开发管理
-[RDM]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -142,11 +129,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>立项管理
-[PIM]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>系统设计
 [SD]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -162,10 +144,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>项目进度表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>QA周报</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -305,10 +283,6 @@
     <t>发布</t>
   </si>
   <si>
-    <t>发布</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CCA-PMC-PWR-V1.0.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -341,10 +315,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>可研</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>变更中</t>
   </si>
   <si>
@@ -352,21 +322,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>编码规范</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>质量保证计划</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 实现与测试
-[IT] </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统测试
-[ST]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -396,18 +352,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CCA-PP-PS-V1.0.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CCA-RDM-RFR-V1.0.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">CCA-IT-STD-V1.0.0 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CCA-IT-SDB-V1.0.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -457,6 +405,50 @@
   </si>
   <si>
     <t>杨峻欢</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>立项管理
+[PIM]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求开发管理
+[RDM]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现与测试
+[IT]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统测试
+[ST]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试计划</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCA-ST-SCP-V1.0.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子文档</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>草稿</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -624,7 +616,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -696,10 +688,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -724,27 +712,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1079,57 +1075,57 @@
   <sheetData>
     <row r="1" spans="2:4" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:4" ht="18" customHeight="1">
-      <c r="B2" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="B2" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="2:4" ht="27.95" customHeight="1">
-      <c r="B3" s="28" t="s">
-        <v>40</v>
+      <c r="B3" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="27.95" customHeight="1">
-      <c r="B4" s="29"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="27.95" customHeight="1">
-      <c r="B5" s="29"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="2">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="27.95" customHeight="1">
-      <c r="B6" s="29"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="27.95" customHeight="1">
-      <c r="B7" s="30"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="2">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="43.5" customHeight="1">
@@ -1140,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1156,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1179,10 +1175,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>17</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>6</v>
@@ -1191,13 +1187,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>1</v>
@@ -1212,18 +1208,18 @@
         <v>13</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>24</v>
+      <c r="A2" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
@@ -1231,581 +1227,549 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="25">
-        <v>42095</v>
-      </c>
-      <c r="K2" s="25">
-        <v>42095</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
+      <c r="J2" s="24">
+        <v>42461</v>
+      </c>
+      <c r="K2" s="24">
+        <v>42465</v>
+      </c>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" ht="24" customHeight="1">
+      <c r="A3" s="34"/>
+      <c r="B3" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="25">
-        <v>42095</v>
-      </c>
-      <c r="K3" s="25">
-        <v>42099</v>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24">
+        <v>42468</v>
+      </c>
+      <c r="K3" s="24">
+        <v>42475</v>
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>32</v>
+    <row r="4" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" ht="20.25" customHeight="1">
+      <c r="A7" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="24">
+        <v>42461</v>
+      </c>
+      <c r="K7" s="24">
+        <v>42461</v>
+      </c>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A9" s="34"/>
+      <c r="B9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25">
-        <v>42102</v>
-      </c>
-      <c r="K4" s="25">
-        <v>42109</v>
-      </c>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="25">
-        <v>42102</v>
-      </c>
-      <c r="K5" s="25">
-        <v>42109</v>
-      </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A8" s="32"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="25">
-        <v>42095</v>
-      </c>
-      <c r="K9" s="25">
-        <v>42095</v>
-      </c>
+      <c r="J9" s="24">
+        <v>42461</v>
+      </c>
+      <c r="K9" s="9"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
+    <row r="10" spans="1:12">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="24">
+        <v>42468</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24">
+        <v>42482</v>
+      </c>
+      <c r="K11" s="24">
+        <v>42482</v>
+      </c>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A12" s="34"/>
+      <c r="B12" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="25">
-        <v>42095</v>
-      </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="H12" s="7"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="25">
-        <v>42102</v>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24">
+        <v>42482</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="6" t="s">
-        <v>56</v>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>43</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25">
-        <v>42116</v>
-      </c>
-      <c r="K13" s="25">
-        <v>42116</v>
+      <c r="I13" s="8"/>
+      <c r="J13" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="32"/>
-      <c r="B14" s="31" t="s">
-        <v>78</v>
+    <row r="14" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A14" s="34"/>
+      <c r="B14" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>64</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25">
-        <v>42109</v>
-      </c>
-      <c r="K14" s="25">
-        <v>42109</v>
+      <c r="I14" s="8"/>
+      <c r="J14" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
+    <row r="15" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="9" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>80</v>
+        <v>94</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="24"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="25">
-        <v>42116</v>
-      </c>
-      <c r="K15" s="9"/>
+        <v>42475</v>
+      </c>
+      <c r="K15" s="25">
+        <v>42485</v>
+      </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>82</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="J16" s="24">
+        <v>42524</v>
+      </c>
+      <c r="K16" s="9"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32" t="s">
+      <c r="A17" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24">
+        <v>42475</v>
+      </c>
+      <c r="K17" s="24">
+        <v>42475</v>
+      </c>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="25">
-        <v>42158</v>
-      </c>
-      <c r="K18" s="9"/>
+      <c r="K18" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="34" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="23"/>
+      <c r="J19" s="24">
+        <v>42475</v>
+      </c>
+      <c r="K19" s="24">
+        <v>42475</v>
+      </c>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24">
+        <v>42475</v>
+      </c>
+      <c r="K20" s="24">
+        <v>42475</v>
+      </c>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25">
-        <v>42109</v>
-      </c>
-      <c r="K19" s="25">
-        <v>42109</v>
-      </c>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="D21" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="25">
-        <v>42109</v>
-      </c>
-      <c r="K21" s="25">
-        <v>42109</v>
+        <v>87</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25">
-        <v>42109</v>
-      </c>
-      <c r="K22" s="25">
-        <v>42109</v>
-      </c>
-      <c r="L22" s="7"/>
+      <c r="C22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="11"/>
+      <c r="L22" s="12"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="K23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="L23" s="7"/>
+      <c r="C23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="11"/>
+      <c r="L23" s="12"/>
     </row>
     <row r="24" spans="1:12">
       <c r="C24" s="12"/>
@@ -1942,45 +1906,25 @@
       <c r="I38" s="11"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="3:12">
-      <c r="C39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="11"/>
-      <c r="L39" s="12"/>
-    </row>
-    <row r="40" spans="3:12">
-      <c r="C40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="11"/>
-      <c r="L40" s="12"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A9:A18"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:F23 F15:F17 F2:F10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19:F21 F12:F15 F2:F8">
       <formula1>"纸质文档,电子文档,其他"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21">
       <formula1>"草稿,发布,正在修改,变更中"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2012,20 +1956,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="24">
       <c r="A2" s="17" t="s">
@@ -2035,16 +1979,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>7</v>

</xml_diff>